<commit_message>
Modifying the appearance of the errors boxes
</commit_message>
<xml_diff>
--- a/crop_prices.xlsx
+++ b/crop_prices.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RTV-LPT1-233\Desktop\edison jupyter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edison New\Desktop\edison jupyter\quality checks folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809D0CC1-F63F-4C35-846C-08E70819BA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF079C2-BD7B-4059-A274-C35094735199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2C928138-B423-4FF9-A5F2-703B011EA9CC}"/>
   </bookViews>
@@ -877,7 +877,7 @@
   <dimension ref="A1:C162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1368,7 +1368,7 @@
         <v>20000</v>
       </c>
       <c r="C44">
-        <v>150000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1379,7 +1379,7 @@
         <v>20000</v>
       </c>
       <c r="C45">
-        <v>150000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>